<commit_message>
Pega works now with proper numbers
</commit_message>
<xml_diff>
--- a/AddClient.xlsx
+++ b/AddClient.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Bradburn_K-P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D1122B-478E-4CEE-B467-070E70E4BF39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EC12EE-0375-43F2-9B85-DACE61B244FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="1635" windowWidth="38700" windowHeight="15435" xr2:uid="{C8735221-E8B6-42D6-A887-96FF16360338}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>Store</t>
   </si>
   <si>
-    <t>Kittens</t>
+    <t>Chai</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Running orders now has update info and will not constantly relaunch page.
</commit_message>
<xml_diff>
--- a/AddClient.xlsx
+++ b/AddClient.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Bradburn_K-P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EC12EE-0375-43F2-9B85-DACE61B244FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA7C5A4-CAB4-4864-A413-3D270CB278E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="1635" windowWidth="38700" windowHeight="15435" xr2:uid="{C8735221-E8B6-42D6-A887-96FF16360338}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Chai</t>
+  </si>
+  <si>
+    <t>Northwoods Cranberry Sauce</t>
   </si>
 </sst>
 </file>
@@ -412,15 +415,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A99433E-F547-4662-8035-A4DFF952560B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -479,6 +483,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Emailed Reciepts stretch goal.
</commit_message>
<xml_diff>
--- a/AddClient.xlsx
+++ b/AddClient.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth Bradburn\Documents\UiPath\Bradburn_K-P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA7C5A4-CAB4-4864-A413-3D270CB278E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D7149-DB3A-4544-96C3-4837F1599390}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1635" windowWidth="38700" windowHeight="15435" xr2:uid="{C8735221-E8B6-42D6-A887-96FF16360338}"/>
+    <workbookView minimized="1" xWindow="3630" yWindow="1635" windowWidth="25170" windowHeight="15435" activeTab="1" xr2:uid="{C8735221-E8B6-42D6-A887-96FF16360338}"/>
   </bookViews>
   <sheets>
     <sheet name="Sarah" sheetId="1" r:id="rId1"/>
+    <sheet name="Expense" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -64,6 +65,42 @@
   </si>
   <si>
     <t>Northwoods Cranberry Sauce</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Emma_email</t>
+  </si>
+  <si>
+    <t>Taco</t>
+  </si>
+  <si>
+    <t>Tammy</t>
+  </si>
+  <si>
+    <t>Tammy_email</t>
+  </si>
+  <si>
+    <t>clientid</t>
+  </si>
+  <si>
+    <t>clientname</t>
+  </si>
+  <si>
+    <t>clientemail</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>subtotal</t>
   </si>
 </sst>
 </file>
@@ -417,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A99433E-F547-4662-8035-A4DFF952560B}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,4 +537,203 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7157A983-E587-4402-A78F-33CE845D72B6}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>3.5</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>281</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>281</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>281</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>3.5</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>281</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>